<commit_message>
update excel from google drive
</commit_message>
<xml_diff>
--- a/rtl/user/doc/Interface-Definition.xlsx
+++ b/rtl/user/doc/Interface-Definition.xlsx
@@ -320,7 +320,11 @@
 wb_clk</t>
   </si>
   <si>
-    <t>io_in:38</t>
+    <t>io_in:38,
+vccd1,
+vccd2,
+vssd1,
+vssd2</t>
   </si>
   <si>
     <t>PRIMARY_OUTPUT</t>

</xml_diff>

<commit_message>
change FSIC_MISC to FSIC_CLKRST, add basic logic in it
</commit_message>
<xml_diff>
--- a/rtl/user/doc/Interface-Definition.xlsx
+++ b/rtl/user/doc/Interface-Definition.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="346">
   <si>
     <t>Interface</t>
   </si>
@@ -116,7 +116,7 @@
 (Kerwin)</t>
   </si>
   <si>
-    <t>FSIC_MISC
+    <t>FSIC_CLKRST
 (Patrick)</t>
   </si>
   <si>
@@ -289,6 +289,9 @@
     <t>user_prj_sel : 5</t>
   </si>
   <si>
+    <t>mb_irq</t>
+  </si>
+  <si>
     <t>user_prj_irq</t>
   </si>
   <si>
@@ -337,9 +340,11 @@
     <t>la_data_out:128</t>
   </si>
   <si>
+    <t>user_irq:3</t>
+  </si>
+  <si>
     <t>io_out:38,
-io_oeb:38,
-user_irq:3</t>
+io_oeb:38</t>
   </si>
   <si>
     <r>
@@ -6059,12 +6064,14 @@
       <c r="B9" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="15"/>
+      <c r="C9" s="15" t="s">
+        <v>54</v>
+      </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>31</v>
@@ -6075,7 +6082,7 @@
     </row>
     <row r="10">
       <c r="A10" s="11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>53</v>
@@ -6083,7 +6090,7 @@
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
       <c r="E10" s="13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
@@ -6103,204 +6110,204 @@
     </row>
     <row r="12">
       <c r="A12" s="22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C12" s="23"/>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
       <c r="F12" s="15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G12" s="24"/>
       <c r="H12" s="25" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I12" s="25" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
       <c r="F13" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G13" s="26"/>
-      <c r="H13" s="25"/>
+      <c r="H13" s="14" t="s">
+        <v>66</v>
+      </c>
       <c r="I13" s="25" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="27" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
       <c r="E14" s="23" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G14" s="24"/>
       <c r="H14" s="28" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I14" s="28" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="27" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D15" s="23"/>
       <c r="E15" s="23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H15" s="28" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I15" s="28" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="F16" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="G16" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="H16" s="28" t="s">
-        <v>69</v>
-      </c>
       <c r="I16" s="28" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="27" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B17" s="23"/>
       <c r="C17" s="23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H17" s="28" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I17" s="28" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="27" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B18" s="23"/>
       <c r="C18" s="23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H18" s="28" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I18" s="28" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="22" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="H19" s="15" t="s">
-        <v>75</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="H19" s="15"/>
       <c r="I19" s="15" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20">
@@ -9259,156 +9266,156 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="31" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B2" s="31">
         <v>1.0</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="31" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B3" s="31">
         <v>1.0</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="31" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B4" s="31">
         <v>32.0</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="31" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B5" s="31">
         <v>32.0</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="31" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B6" s="31">
         <v>4.0</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="31" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B7" s="31">
         <v>1.0</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="31" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B8" s="31">
         <v>1.0</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B9" s="31">
         <v>1.0</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="31" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B10" s="31">
         <v>1.0</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="31" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B11" s="31">
         <v>32.0</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12">
@@ -9463,44 +9470,44 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="33" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B2" s="33">
         <v>7.0</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="33" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B3" s="33">
         <v>7.0</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -9526,315 +9533,315 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="33" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B2" s="33">
         <v>1.0</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="33" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B3" s="33">
         <v>1.0</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="33" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B4" s="33">
         <v>1.0</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="33" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B5" s="33">
         <v>1.0</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="33" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B6" s="33">
         <v>1.0</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="33" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B7" s="33">
         <v>32.0</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="33" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B8" s="33">
         <v>4.0</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="33" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B9" s="33">
         <v>4.0</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="33" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B10" s="33">
         <v>1.0</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="33" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B11" s="33">
         <v>2.0</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="33" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B12" s="33">
         <v>0.0</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="33" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B13" s="33">
         <v>2.0</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="33" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B14" s="33">
         <v>1.0</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="33" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B15" s="33">
         <v>1.0</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="33" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B16" s="33">
         <v>32.0</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="33" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B17" s="33">
         <v>4.0</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="33" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B18" s="33">
         <v>4.0</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="33" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B19" s="33">
         <v>1.0</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="33" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B20" s="33">
         <v>2.0</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D20" s="33" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="33" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B21" s="33">
         <v>0.0</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="33" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B22" s="33">
         <v>2.0</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D22" s="33" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="34" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B26" s="35">
         <f>sum(B5:B13)</f>
@@ -9842,12 +9849,12 @@
       </c>
       <c r="C26" s="35"/>
       <c r="D26" s="34" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="34" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B27" s="35">
         <f>sum(B14:B22)</f>
@@ -9855,7 +9862,7 @@
       </c>
       <c r="C27" s="35"/>
       <c r="D27" s="34" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -9881,306 +9888,306 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="33" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="34" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B3" s="33">
         <v>1.0</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="34" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B4" s="33">
         <v>1.0</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="33" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B5" s="33">
         <v>1.0</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="33" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B6" s="33">
         <v>1.0</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="33" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B7" s="33">
         <v>32.0</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="33" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B8" s="33">
         <v>4.0</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="33" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B9" s="33">
         <v>4.0</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="33" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B10" s="33">
         <v>1.0</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="33" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B11" s="33">
         <v>2.0</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="33" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B12" s="33">
         <v>2.0</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="33" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="34" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B14" s="33">
         <v>1.0</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="34" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B15" s="33">
         <v>1.0</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="33" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B16" s="33">
         <v>1.0</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="33" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B17" s="33">
         <v>1.0</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="33" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B18" s="33">
         <v>32.0</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="33" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B19" s="33">
         <v>4.0</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="33" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B20" s="33">
         <v>4.0</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D20" s="33" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="33" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B21" s="33">
         <v>1.0</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="33" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B22" s="33">
         <v>2.0</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D22" s="33" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="33" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B23" s="33">
         <v>2.0</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D23" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -10206,521 +10213,521 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="33" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="34" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B3" s="33">
         <v>1.0</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="34" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B4" s="33">
         <v>1.0</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="33" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B5" s="33">
         <v>1.0</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="33" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B6" s="33">
         <v>1.0</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="33" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B7" s="33">
         <v>12.0</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="33" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B8" s="33">
         <v>1.0</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="33" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B9" s="33">
         <v>1.0</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="33" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B10" s="33">
         <v>32.0</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="33" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B11" s="33">
         <v>4.0</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="33" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B12" s="33">
         <v>1.0</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="33" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B13" s="33">
         <v>1.0</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="33" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B14" s="33">
         <v>12.0</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="33" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B15" s="33">
         <v>1.0</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="33" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B16" s="33">
         <v>1.0</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="33" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B17" s="33">
         <v>32.0</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="33" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="34" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B19" s="33">
         <v>1.0</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="34" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B20" s="33">
         <v>1.0</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D20" s="33" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="33" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B21" s="33">
         <v>1.0</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="33" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B22" s="33">
         <v>1.0</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D22" s="33" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="33" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B23" s="33">
         <v>12.0</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D23" s="33" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="33" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B24" s="33">
         <v>1.0</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D24" s="33" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="33" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B25" s="33">
         <v>1.0</v>
       </c>
       <c r="C25" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D25" s="33" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="33" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B26" s="33">
         <v>32.0</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D26" s="33" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="33" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B27" s="33">
         <v>4.0</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D27" s="33" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="33" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B28" s="33">
         <v>1.0</v>
       </c>
       <c r="C28" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D28" s="33" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="33" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B29" s="33">
         <v>1.0</v>
       </c>
       <c r="C29" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D29" s="33" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="33" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B30" s="33">
         <v>12.0</v>
       </c>
       <c r="C30" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D30" s="33" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="33" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B31" s="33">
         <v>1.0</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D31" s="33" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="33" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B32" s="33">
         <v>1.0</v>
       </c>
       <c r="C32" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D32" s="33" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="33" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B33" s="33">
         <v>32.0</v>
       </c>
       <c r="C33" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D33" s="33" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="33" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="33" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B35" s="34">
         <v>28.0</v>
       </c>
       <c r="C35" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D35" s="33" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="33" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B36" s="34">
         <v>32.0</v>
       </c>
       <c r="C36" s="33" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D36" s="33" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="33" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B37" s="34">
         <v>32.0</v>
       </c>
       <c r="C37" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D37" s="33" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="33" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B38" s="33">
         <v>1.0</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D38" s="33" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="33" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B39" s="33">
         <v>1.0</v>
       </c>
       <c r="C39" s="33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D39" s="33" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -10746,612 +10753,612 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="36" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B2" s="36">
         <v>1.0</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="36" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B3" s="36">
         <v>1.0</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="36" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B4" s="36">
         <v>1.0</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="36" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B5" s="38">
         <v>64.0</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="36" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B6" s="36">
         <v>1.0</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="38" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B7" s="36">
         <v>1.0</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="38" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B8" s="36">
         <v>1.0</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="39" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B9" s="36">
         <v>32.0</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="39" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B10" s="36">
         <v>1.0</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="39" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B11" s="36">
         <v>1.0</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="39" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B12" s="36">
         <v>32.0</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="39" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B13" s="36">
         <v>4.0</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="39" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B14" s="36">
         <v>1.0</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="39" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B15" s="36">
         <v>1.0</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D15" s="36" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="39" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B16" s="36">
         <v>2.0</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D16" s="36" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="39" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B17" s="36">
         <v>1.0</v>
       </c>
       <c r="C17" s="36" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D17" s="36" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="39" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B18" s="36">
         <v>1.0</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D18" s="36" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="39" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B19" s="36">
         <v>32.0</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D19" s="36" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="39" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B20" s="36">
         <v>1.0</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D20" s="36" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="39" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B21" s="36">
         <v>1.0</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="39" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B22" s="36">
         <v>32.0</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D22" s="36" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="39" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B23" s="36">
         <v>2.0</v>
       </c>
       <c r="C23" s="36" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D23" s="36" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="39" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B24" s="36">
         <v>1.0</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D24" s="36" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="40" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B25" s="36">
         <v>1.0</v>
       </c>
       <c r="C25" s="37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D25" s="41" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="38" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B26" s="36">
         <v>1.0</v>
       </c>
       <c r="C26" s="36" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="38" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B27" s="36">
         <v>1.0</v>
       </c>
       <c r="C27" s="37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="36" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B28" s="36">
         <v>1.0</v>
       </c>
       <c r="C28" s="36" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D28" s="36" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="36" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B29" s="36">
         <v>1.0</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D29" s="36" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="36" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B30" s="36">
         <v>32.0</v>
       </c>
       <c r="C30" s="36" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D30" s="36" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="36" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B31" s="36"/>
       <c r="C31" s="36" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D31" s="36" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="36" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B32" s="36"/>
       <c r="C32" s="36" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D32" s="36" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="36" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B33" s="36">
         <v>1.0</v>
       </c>
       <c r="C33" s="36" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D33" s="36" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="36" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B34" s="36"/>
       <c r="C34" s="36" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D34" s="36" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="36" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B35" s="36"/>
       <c r="C35" s="36" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D35" s="36" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="36" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B36" s="36"/>
       <c r="C36" s="36" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D36" s="36" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="36" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B37" s="36">
         <v>1.0</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D37" s="36" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="36" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B38" s="36">
         <v>1.0</v>
       </c>
       <c r="C38" s="36" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D38" s="36" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="36" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B39" s="36">
         <v>32.0</v>
       </c>
       <c r="C39" s="37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D39" s="36" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="36" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B40" s="42"/>
       <c r="C40" s="37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D40" s="36" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="36" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B41" s="42"/>
       <c r="C41" s="37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="36" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B42" s="36">
         <v>1.0</v>
       </c>
       <c r="C42" s="37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D42" s="36" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="36" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B43" s="42"/>
       <c r="C43" s="37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D43" s="36" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="36" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B44" s="42"/>
       <c r="C44" s="37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D44" s="36" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="36" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B45" s="42"/>
       <c r="C45" s="37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D45" s="36" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>